<commit_message>
Updated logbook for Sprint #2
</commit_message>
<xml_diff>
--- a/docs/logbooks/MBlaul - Efforts Logbook.xlsx
+++ b/docs/logbooks/MBlaul - Efforts Logbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Matt\Documents\GitHub\skypi\docs\logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE348BAF-F8CD-4457-8C24-C2C926C28C58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BD5357D-AF0B-44CE-A0E9-02B1261DB05B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -169,22 +169,26 @@
 Presentation</t>
   </si>
   <si>
-    <t>A, B, C, H, I, J, M, N, L</t>
-  </si>
-  <si>
-    <t>Configuring mongodb/cloud server, deploying app to cloud platform, user roles and auth, training users on API</t>
-  </si>
-  <si>
     <t>Architecture,
 Project Plan Update,
 Configurations,
 Deployment</t>
   </si>
   <si>
-    <t>github.com/mblaul/skypi/api</t>
-  </si>
-  <si>
-    <t>/core/api/models/User.js,
+    <t>Configuring mongodb/cloud server, deploying app to cloud platform, user roles and auth, training users on API, installed additional security protocols</t>
+  </si>
+  <si>
+    <t>A, B, C, E, F, H, I, J, L, M, N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">github.com/mblaul/skypi/api,
+Google Team Drive,
+Postman Documentation
+</t>
+  </si>
+  <si>
+    <t>/core/api/*,
+/core/api/models/User.js,
 /core/api/models/Weather.js,
 /core/api/controllers/user.js,
 /core/api/controllers/weather.js</t>
@@ -388,6 +392,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -400,40 +428,16 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -718,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -735,40 +739,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="17" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="27"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="26"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
@@ -789,10 +793,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="24"/>
       <c r="C4" s="11">
         <v>12</v>
       </c>
@@ -811,21 +815,21 @@
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="21"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="14">
         <v>20</v>
       </c>
       <c r="D5" s="14" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>45</v>
       </c>
       <c r="F5" s="16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G5" s="16" t="s">
         <v>47</v>
@@ -835,10 +839,10 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="21"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
       <c r="E6" s="2"/>
@@ -847,10 +851,10 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="21"/>
+      <c r="B7" s="18"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="2"/>
@@ -859,10 +863,10 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="21"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -871,10 +875,10 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -883,10 +887,10 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -895,10 +899,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="18"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -907,10 +911,10 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="21" t="s">
+      <c r="A12" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="21"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -919,10 +923,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="21"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="2"/>
@@ -931,10 +935,10 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="21"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="2"/>
@@ -943,10 +947,10 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
+      <c r="A15" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="21"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
@@ -956,6 +960,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -969,11 +978,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -983,8 +987,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -997,68 +1001,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="22" t="s">
+      <c r="B2" s="21"/>
+      <c r="C2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="23"/>
-      <c r="K2" s="23"/>
-      <c r="L2" s="23"/>
-      <c r="M2" s="23"/>
-      <c r="N2" s="23"/>
-      <c r="O2" s="23"/>
-      <c r="P2" s="24"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="29"/>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
-      <c r="J3" s="29"/>
-      <c r="K3" s="29"/>
-      <c r="L3" s="29"/>
-      <c r="M3" s="29"/>
-      <c r="N3" s="29"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="29"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="32"/>
+      <c r="M3" s="32"/>
+      <c r="N3" s="32"/>
+      <c r="O3" s="32"/>
+      <c r="P3" s="32"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1112,7 +1116,7 @@
     </row>
     <row r="5" spans="1:16" s="3" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>38</v>
@@ -1149,8 +1153,8 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="32">
-        <v>1</v>
+      <c r="A6" s="17">
+        <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>38</v>
@@ -1159,36 +1163,40 @@
         <v>1</v>
       </c>
       <c r="D6" s="8">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10">
+        <v>3</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
         <v>2</v>
-      </c>
-      <c r="E6" s="10">
-        <v>1</v>
-      </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8">
-        <v>1</v>
       </c>
       <c r="I6" s="8"/>
       <c r="J6" s="8">
+        <v>1</v>
+      </c>
+      <c r="K6" s="8">
+        <v>6</v>
+      </c>
+      <c r="L6" s="8">
         <v>2</v>
-      </c>
-      <c r="K6" s="8">
-        <v>4</v>
-      </c>
-      <c r="L6" s="8">
-        <v>1</v>
       </c>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
+      <c r="O6" s="8">
+        <v>1</v>
+      </c>
       <c r="P6" s="8">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -1208,7 +1216,7 @@
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -1228,7 +1236,7 @@
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -1248,7 +1256,7 @@
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -1268,7 +1276,7 @@
     </row>
     <row r="11" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -1288,7 +1296,7 @@
     </row>
     <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -1308,7 +1316,7 @@
     </row>
     <row r="13" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -1327,8 +1335,8 @@
       <c r="P13" s="2"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="16"/>

</xml_diff>

<commit_message>
Adding some backend logic for verification of accounts, fixed bug relating to that on frontend, also updated logbook
</commit_message>
<xml_diff>
--- a/docs/logbooks/MBlaul - Efforts Logbook.xlsx
+++ b/docs/logbooks/MBlaul - Efforts Logbook.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Matt\Documents\GitHub\skypi\docs\logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{631AE6C7-014A-43F9-9792-DF56C350BEBC}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725ECEE6-83AC-49FB-86E5-9A48C5457393}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -194,7 +194,32 @@
 /core/api/controllers/weather.js</t>
   </si>
   <si>
-    <t>10/4 - Coded react front end, group communication, tardec visit</t>
+    <t>Architecture,
+Project Plan Update,
+User Interface Design, User Stories, Tools Tech ETC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/core/api/*,
+/frontend/client/src/App,
+/frontend/client/src/compenents/layout/Navbar,
+/frontend/client/src/compenents/authentication/Login,
+/frontend/client/src/compenents/authentication/Register,
+/frontend/client/src/compenents/content/Landing
+</t>
+  </si>
+  <si>
+    <t>github.com/mblaul/skypi/api,
+github.com/mblaul/skypi/frontend,
+Google Team Drive,
+https://drive.google.com/drive/u/1/folders/0ADmYitmSMBPCUk9PVA
+Team Trello,
+https://trello.com/skypitasksseniordesign/home</t>
+  </si>
+  <si>
+    <t>A, B, C, D, E, F, H, I, J, M, N</t>
+  </si>
+  <si>
+    <t>Coded react front end, group communication,  Coordinated with group and assigned tasks, two group meetings, researched bootstrap landing pages, Stakeholder meeting with TARDEC</t>
   </si>
 </sst>
 </file>
@@ -351,7 +376,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -398,6 +423,30 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -409,27 +458,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -725,8 +753,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -737,45 +765,45 @@
     <col min="4" max="4" width="27.5" customWidth="1"/>
     <col min="5" max="5" width="42.5" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="28" customWidth="1"/>
+    <col min="7" max="7" width="33.125" customWidth="1"/>
+    <col min="8" max="8" width="51.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="27"/>
+      <c r="H2" s="28"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="27"/>
+      <c r="B3" s="24"/>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
@@ -796,10 +824,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="28"/>
+      <c r="B4" s="25"/>
       <c r="C4" s="11">
         <v>12</v>
       </c>
@@ -812,16 +840,16 @@
       <c r="F4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="16" t="s">
         <v>40</v>
       </c>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="22"/>
+      <c r="B5" s="19"/>
       <c r="C5" s="14">
         <v>20</v>
       </c>
@@ -841,27 +869,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+    <row r="6" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+      <c r="A6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="5">
-        <v>7</v>
-      </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="2" t="s">
+      <c r="B6" s="19"/>
+      <c r="C6" s="18">
+        <v>18</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="G6" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="22"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
       <c r="E7" s="2"/>
@@ -870,10 +906,10 @@
       <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="22"/>
+      <c r="B8" s="19"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -882,10 +918,10 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="22"/>
+      <c r="B9" s="19"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -894,10 +930,10 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="22"/>
+      <c r="B10" s="19"/>
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
       <c r="E10" s="2"/>
@@ -906,10 +942,10 @@
       <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="22"/>
+      <c r="B11" s="19"/>
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
       <c r="E11" s="2"/>
@@ -918,10 +954,10 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="22"/>
+      <c r="B12" s="19"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="2"/>
@@ -930,10 +966,10 @@
       <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="22" t="s">
+      <c r="A13" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="22"/>
+      <c r="B13" s="19"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
       <c r="E13" s="2"/>
@@ -942,10 +978,10 @@
       <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
+      <c r="A14" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="22"/>
+      <c r="B14" s="19"/>
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="2"/>
@@ -954,10 +990,10 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="22" t="s">
+      <c r="A15" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="22"/>
+      <c r="B15" s="19"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="2"/>
@@ -967,6 +1003,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
@@ -980,11 +1021,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -994,8 +1030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1008,68 +1044,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="23" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="25"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="31"/>
-      <c r="B3" s="31"/>
-      <c r="C3" s="32" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="32"/>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="32"/>
-      <c r="M3" s="32"/>
-      <c r="N3" s="32"/>
-      <c r="O3" s="32"/>
-      <c r="P3" s="32"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1202,24 +1238,48 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7">
+      <c r="A7" s="17">
         <v>3</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
+      <c r="B7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8">
+        <v>3</v>
+      </c>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
+      <c r="F7" s="8">
+        <v>5</v>
+      </c>
+      <c r="G7" s="8">
+        <v>1</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8">
+        <v>1</v>
+      </c>
+      <c r="K7" s="8">
+        <v>3</v>
+      </c>
+      <c r="L7" s="8">
+        <v>1</v>
+      </c>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="8">
+        <v>1</v>
+      </c>
+      <c r="P7" s="8">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
@@ -1342,8 +1402,8 @@
       <c r="P13" s="2"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="16"/>

</xml_diff>

<commit_message>
Admin page not working, this commit is so I can work from my desktop
</commit_message>
<xml_diff>
--- a/docs/logbooks/MBlaul - Efforts Logbook.xlsx
+++ b/docs/logbooks/MBlaul - Efforts Logbook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Matt\Documents\GitHub\skypi\docs\logbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mblau\Documents\GitHub\skypi\docs\logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725ECEE6-83AC-49FB-86E5-9A48C5457393}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883367E1-C7BF-4808-AD7F-37476D5935F0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Example" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -125,24 +125,6 @@
   </si>
   <si>
     <t>Sprint # 6</t>
-  </si>
-  <si>
-    <t>Sprint # 7</t>
-  </si>
-  <si>
-    <t>Sprint # 8</t>
-  </si>
-  <si>
-    <t>Sprint # 9</t>
-  </si>
-  <si>
-    <t>Sprint # 10</t>
-  </si>
-  <si>
-    <t>Sprint # 11</t>
-  </si>
-  <si>
-    <t>Sprint # 12</t>
   </si>
   <si>
     <t>Matt Blaul</t>
@@ -220,6 +202,20 @@
   </si>
   <si>
     <t>Coded react front end, group communication,  Coordinated with group and assigned tasks, two group meetings, researched bootstrap landing pages, Stakeholder meeting with TARDEC</t>
+  </si>
+  <si>
+    <t>Coordinated with group and assigned tasks, two group meetings, implemented device favoriting, user verification, admin routes/links, added stations/station page, added Last Updated to Dashboard page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/core/api/*,
+/frontend/client/src/App,
+/frontend/client/src/compenents/authentication/Verify,
+/frontend/client/src/compenents/content/dashboard/Dashboard,
+/frontend/client/src/compenents/content/stations/Stations,
+/frontend/client/src/compenents/content/station/Station,
+/frontend/client/src/actions/*
+/frontend/client/src/reducers/*
+</t>
   </si>
 </sst>
 </file>
@@ -415,9 +411,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -427,6 +420,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -446,18 +454,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -486,6 +482,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>666020</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28005</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{129685D7-AD38-43BA-868B-B111AEC0C8BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4657725" y="4267200"/>
+          <a:ext cx="5838095" cy="4561905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -751,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -766,44 +811,44 @@
     <col min="5" max="5" width="42.5" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="33.125" customWidth="1"/>
-    <col min="8" max="8" width="51.875" customWidth="1"/>
+    <col min="8" max="8" width="55.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="26" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="27"/>
-      <c r="H2" s="28"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="24"/>
+      <c r="B3" s="28"/>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
@@ -824,92 +869,104 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="25"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="11">
         <v>12</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G4" s="16" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="H4" s="13"/>
     </row>
     <row r="5" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="19"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="14">
         <v>20</v>
       </c>
       <c r="D5" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="126" x14ac:dyDescent="0.25">
+      <c r="A6" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="17">
+        <v>18</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E6" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="H6" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="H5" s="16" t="s">
+    </row>
+    <row r="7" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="23"/>
+      <c r="C7" s="18">
+        <v>24</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="15" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="126" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="18">
-        <v>18</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="16" t="s">
+      <c r="F7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="19"/>
+      <c r="B8" s="23"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
       <c r="E8" s="2"/>
@@ -918,10 +975,10 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="19"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
@@ -929,98 +986,20 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="B15" s="19"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
+  <mergeCells count="12">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1028,10 +1007,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1049,7 +1028,7 @@
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="30" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D1" s="30"/>
       <c r="E1" s="30"/>
@@ -1066,26 +1045,26 @@
       <c r="P1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="22"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="26"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32"/>
@@ -1162,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C5" s="8">
         <v>1</v>
@@ -1196,11 +1175,11 @@
       </c>
     </row>
     <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17">
+      <c r="A6" s="16">
         <v>2</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C6" s="8">
         <v>1</v>
@@ -1238,11 +1217,11 @@
       </c>
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="17">
+      <c r="A7" s="16">
         <v>3</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="C7" s="8">
         <v>1</v>
@@ -1282,24 +1261,48 @@
       </c>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7">
+      <c r="A8" s="16">
         <v>4</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
+      <c r="B8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="8">
+        <v>2</v>
+      </c>
+      <c r="E8" s="10">
+        <v>2</v>
+      </c>
+      <c r="F8" s="8">
+        <v>4</v>
+      </c>
+      <c r="G8" s="8">
+        <v>1</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8">
+        <v>2</v>
+      </c>
+      <c r="K8" s="8">
+        <v>4</v>
+      </c>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="8">
+        <v>1</v>
+      </c>
+      <c r="P8" s="8">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
@@ -1341,86 +1344,16 @@
       <c r="O10" s="2"/>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <v>7</v>
-      </c>
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-    </row>
-    <row r="12" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>8</v>
-      </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-    </row>
-    <row r="13" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>9</v>
-      </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="16"/>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="15"/>
-    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="6">
     <mergeCell ref="C1:P1"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="B17:C17"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:P2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="C3:P3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created not found component, still need to route users to it when data/profiles not found
</commit_message>
<xml_diff>
--- a/docs/logbooks/MBlaul - Efforts Logbook.xlsx
+++ b/docs/logbooks/MBlaul - Efforts Logbook.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mblau\Documents\GitHub\skypi\docs\logbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Matt\Documents\GitHub\skypi\docs\logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883367E1-C7BF-4808-AD7F-37476D5935F0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A103A7-251A-42DB-9A6B-52BE54219893}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -215,6 +215,23 @@
 /frontend/client/src/compenents/content/station/Station,
 /frontend/client/src/actions/*
 /frontend/client/src/reducers/*
+</t>
+  </si>
+  <si>
+    <t>Group meetings, assigned tasks, worked on backend getting data by data, search functionality for data by locations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/core/api/controllers/weather.js,
+/core/api/routes/weather.js,
+/frontend/client/src/App.js,
+/frontend/client/src/compenents/content/dashboard/Dashboard.js,
+/frontend/client/src/compenents/content/station/Station.js,
+/frontend/client/src/compenents/content/station/Location.js,
+/frontend/client/src/compenents/content/station/Locations.js,
+/frontend/client/src/compenents/content/user/Settings.js,
+/frontend/client/src/actions/weatherActions.js,
+/frontend/client/src/reducers/weatherRedcuer.js,
+/frontend/client/src/actions/weatherActions.js,
 </t>
   </si>
 </sst>
@@ -372,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -422,6 +439,30 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -433,27 +474,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -798,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -811,44 +831,44 @@
     <col min="5" max="5" width="42.5" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
     <col min="7" max="7" width="33.125" customWidth="1"/>
-    <col min="8" max="8" width="55.75" customWidth="1"/>
+    <col min="8" max="8" width="71.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="19" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="28"/>
+      <c r="H2" s="29"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="25"/>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
@@ -869,10 +889,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="29" t="s">
+      <c r="A4" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="29"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="11">
         <v>12</v>
       </c>
@@ -962,17 +982,29 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="267.75" x14ac:dyDescent="0.25">
       <c r="A8" s="23" t="s">
         <v>30</v>
       </c>
       <c r="B8" s="23"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="C8" s="19">
+        <v>16</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="H8" s="15" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="23" t="s">
@@ -988,6 +1020,9 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A8:B8"/>
@@ -997,9 +1032,6 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1009,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1023,68 +1055,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
-      <c r="I1" s="30"/>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="30"/>
-      <c r="P1" s="30"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
+      <c r="O1" s="31"/>
+      <c r="P1" s="31"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="24" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="26"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="21"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="22"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="32"/>
-      <c r="B3" s="32"/>
-      <c r="C3" s="33" t="s">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -1308,21 +1340,45 @@
       <c r="A9" s="7">
         <v>5</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
+      <c r="B9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="8">
+        <v>1</v>
+      </c>
+      <c r="E9" s="10">
+        <v>1</v>
+      </c>
+      <c r="F9" s="8">
+        <v>3</v>
+      </c>
+      <c r="G9" s="8">
+        <v>2</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8">
+        <v>2</v>
+      </c>
+      <c r="K9" s="8">
+        <v>3</v>
+      </c>
+      <c r="L9" s="8">
+        <v>1</v>
+      </c>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8">
+        <v>1</v>
+      </c>
+      <c r="P9" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7">

</xml_diff>

<commit_message>
New favicon, more branding, cleaning up landing page
</commit_message>
<xml_diff>
--- a/docs/logbooks/MBlaul - Efforts Logbook.xlsx
+++ b/docs/logbooks/MBlaul - Efforts Logbook.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Matt\Documents\GitHub\skypi\docs\logbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A103A7-251A-42DB-9A6B-52BE54219893}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{08F5943E-23F4-4CD5-922C-5469C6277B2B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="55">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -233,6 +233,26 @@
 /frontend/client/src/reducers/weatherRedcuer.js,
 /frontend/client/src/actions/weatherActions.js,
 </t>
+  </si>
+  <si>
+    <t>Group meetings, assigned tasks, worked on polish for the site, user preferences, deployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/core/api/server_https.js
+/core/api/routes/weather.js,
+/frontend/client/src/App.js,
+/frontend/client/src/compenents/content/dashboard/Dashboard.js,
+/frontend/client/src/compenents/content/station/Station.js,
+/frontend/client/src/compenents/content/station/Location.js,
+/frontend/client/src/compenents/content/station/Locations.js,
+/frontend/client/src/compenents/content/station/Map.js,
+/frontend/client/src/compenents/content/user/Settings.js,
+/frontend/client/src/actions/authActions.js,
+/frontend/client/src/reducers/authRedcuer.js
+</t>
+  </si>
+  <si>
+    <t>A, B, C, D, E, F, H, I, J, K, L, M, N</t>
   </si>
 </sst>
 </file>
@@ -389,17 +409,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -442,6 +458,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -462,18 +493,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -819,7 +838,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -835,196 +854,203 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30" t="s">
+      <c r="B1" s="22"/>
+      <c r="C1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="30"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
     </row>
     <row r="2" spans="1:8" ht="41.1" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="27" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="28"/>
-      <c r="H2" s="29"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
     </row>
     <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="4" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="110.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="26" t="s">
+      <c r="A4" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="11">
+      <c r="B4" s="29"/>
+      <c r="C4" s="9">
         <v>12</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="12" t="s">
+      <c r="E4" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="12" t="s">
+      <c r="F4" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H4" s="13"/>
+      <c r="H4" s="11"/>
     </row>
     <row r="5" spans="1:8" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="14">
+      <c r="B5" s="26"/>
+      <c r="C5" s="12">
         <v>20</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="H5" s="15" t="s">
+      <c r="H5" s="13" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="126" x14ac:dyDescent="0.25">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="17">
+      <c r="B6" s="26"/>
+      <c r="C6" s="15">
         <v>18</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H6" s="15" t="s">
+      <c r="H6" s="13" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="173.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="18">
+      <c r="B7" s="26"/>
+      <c r="C7" s="16">
         <v>24</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="13" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="267.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:8" ht="252" x14ac:dyDescent="0.25">
+      <c r="A8" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="19">
+      <c r="B8" s="26"/>
+      <c r="C8" s="17">
         <v>16</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="23" t="s">
+    <row r="9" spans="1:8" ht="236.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="18">
+        <v>20</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>53</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="A2:B2"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A3:B3"/>
@@ -1032,6 +1058,11 @@
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:H1"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A2:B2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1042,7 +1073,7 @@
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1055,350 +1086,378 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="31"/>
-      <c r="N1" s="31"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="31"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
+      <c r="L1" s="30"/>
+      <c r="M1" s="30"/>
+      <c r="N1" s="30"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="30"/>
     </row>
     <row r="2" spans="1:16" ht="41.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="20" t="s">
+      <c r="B2" s="25"/>
+      <c r="C2" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="22"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="25"/>
     </row>
     <row r="3" spans="1:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="34" t="s">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34"/>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="33"/>
+      <c r="H3" s="33"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="33"/>
+      <c r="K3" s="33"/>
+      <c r="L3" s="33"/>
+      <c r="M3" s="33"/>
+      <c r="N3" s="33"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="33"/>
     </row>
     <row r="4" spans="1:16" ht="24" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="G4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="6" t="s">
+      <c r="K4" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L4" s="6" t="s">
+      <c r="L4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="M4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="N4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="P4" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:16" s="3" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
-        <v>1</v>
-      </c>
-      <c r="B5" s="9" t="s">
+    <row r="5" spans="1:16" s="2" customFormat="1" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="8">
-        <v>1</v>
-      </c>
-      <c r="D5" s="8">
+      <c r="C5" s="6">
+        <v>1</v>
+      </c>
+      <c r="D5" s="6">
         <v>2</v>
       </c>
-      <c r="E5" s="10">
-        <v>1</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8">
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6">
         <v>2</v>
       </c>
-      <c r="K5" s="8">
+      <c r="K5" s="6">
         <v>4</v>
       </c>
-      <c r="L5" s="8">
-        <v>1</v>
-      </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8">
+      <c r="L5" s="6">
+        <v>1</v>
+      </c>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="A6" s="14">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="8">
-        <v>1</v>
-      </c>
-      <c r="D6" s="8">
-        <v>1</v>
-      </c>
-      <c r="E6" s="10">
+      <c r="C6" s="6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="6">
+        <v>1</v>
+      </c>
+      <c r="E6" s="8">
         <v>3</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
         <v>2</v>
       </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6">
+        <v>1</v>
+      </c>
+      <c r="K6" s="6">
         <v>6</v>
       </c>
-      <c r="L6" s="8">
+      <c r="L6" s="6">
         <v>2</v>
       </c>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8">
-        <v>1</v>
-      </c>
-      <c r="P6" s="8">
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6">
+        <v>1</v>
+      </c>
+      <c r="P6" s="6">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="A7" s="14">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="8">
-        <v>1</v>
-      </c>
-      <c r="D7" s="8">
+      <c r="C7" s="6">
+        <v>1</v>
+      </c>
+      <c r="D7" s="6">
         <v>3</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <v>3</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="6">
         <v>5</v>
       </c>
-      <c r="G7" s="8">
-        <v>1</v>
-      </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8">
-        <v>1</v>
-      </c>
-      <c r="K7" s="8">
+      <c r="G7" s="6">
+        <v>1</v>
+      </c>
+      <c r="H7" s="6">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6">
+        <v>1</v>
+      </c>
+      <c r="K7" s="6">
         <v>3</v>
       </c>
-      <c r="L7" s="8">
-        <v>1</v>
-      </c>
-      <c r="M7" s="8"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8">
-        <v>1</v>
-      </c>
-      <c r="P7" s="8">
+      <c r="L7" s="6">
+        <v>1</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6">
+        <v>1</v>
+      </c>
+      <c r="P7" s="6">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="A8" s="14">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="8">
-        <v>1</v>
-      </c>
-      <c r="D8" s="8">
+      <c r="C8" s="6">
+        <v>1</v>
+      </c>
+      <c r="D8" s="6">
         <v>2</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>2</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="6">
         <v>4</v>
       </c>
-      <c r="G8" s="8">
-        <v>1</v>
-      </c>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8">
+      <c r="G8" s="6">
+        <v>1</v>
+      </c>
+      <c r="H8" s="6">
+        <v>1</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6">
         <v>2</v>
       </c>
-      <c r="K8" s="8">
+      <c r="K8" s="6">
         <v>4</v>
       </c>
-      <c r="L8" s="8">
-        <v>1</v>
-      </c>
-      <c r="M8" s="8"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8">
-        <v>1</v>
-      </c>
-      <c r="P8" s="8">
+      <c r="L8" s="6">
+        <v>1</v>
+      </c>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6">
+        <v>1</v>
+      </c>
+      <c r="P8" s="6">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7">
+      <c r="A9" s="5">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="8">
-        <v>1</v>
-      </c>
-      <c r="D9" s="8">
-        <v>1</v>
-      </c>
-      <c r="E9" s="10">
-        <v>1</v>
-      </c>
-      <c r="F9" s="8">
+      <c r="C9" s="6">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6">
+        <v>1</v>
+      </c>
+      <c r="E9" s="8">
+        <v>1</v>
+      </c>
+      <c r="F9" s="6">
         <v>3</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="6">
         <v>2</v>
       </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8">
+      <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6">
         <v>2</v>
       </c>
-      <c r="K9" s="8">
+      <c r="K9" s="6">
         <v>3</v>
       </c>
-      <c r="L9" s="8">
-        <v>1</v>
-      </c>
-      <c r="M9" s="8"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8">
-        <v>1</v>
-      </c>
-      <c r="P9" s="8">
+      <c r="L9" s="6">
+        <v>1</v>
+      </c>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6">
+        <v>1</v>
+      </c>
+      <c r="P9" s="6">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="7">
+      <c r="A10" s="5">
         <v>6</v>
       </c>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
+      <c r="B10" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="6">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6">
+        <v>1</v>
+      </c>
+      <c r="E10" s="8">
+        <v>1</v>
+      </c>
+      <c r="F10" s="6">
+        <v>3</v>
+      </c>
+      <c r="G10" s="6">
+        <v>3</v>
+      </c>
+      <c r="H10" s="6">
+        <v>1</v>
+      </c>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6">
+        <v>3</v>
+      </c>
+      <c r="K10" s="6">
+        <v>3</v>
+      </c>
+      <c r="L10" s="6">
+        <v>1</v>
+      </c>
+      <c r="M10" s="6">
+        <v>1</v>
+      </c>
+      <c r="N10" s="6">
+        <v>1</v>
+      </c>
+      <c r="O10" s="6">
+        <v>1</v>
+      </c>
+      <c r="P10" s="6">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>